<commit_message>
New Changes of the Data Scraping!
</commit_message>
<xml_diff>
--- a/DoctorUrl.xlsx
+++ b/DoctorUrl.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naman\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data_Scraping-Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Doctor Url</t>
   </si>
@@ -84,16 +84,29 @@
   </si>
   <si>
     <t>https://kivihealth.com/iam/balveen.singh.3xewj8rp0ouh</t>
+  </si>
+  <si>
+    <t>https://kivihealth.com/iam/mani.dubey.4786</t>
+  </si>
+  <si>
+    <t>https://kivihealth.com/iam/vaibhav.nepalia.3546</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,8 +132,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,100 +430,111 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>